<commit_message>
Update to v1.25 SA
</commit_message>
<xml_diff>
--- a/test/fixtures/files/Sara-Alert-Format-Exposure-Workflow.xlsx
+++ b/test/fixtures/files/Sara-Alert-Format-Exposure-Workflow.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rhack/git/SaraAlert/test/fixtures/files/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/twong/Documents/SARA-ALERT/SaraAlert/test/fixtures/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDE83848-199A-3D42-8139-C01F2EC2EA07}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4570BDC4-1CB0-5743-A4A4-174171637962}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1660" yWindow="2040" windowWidth="21640" windowHeight="14440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="950" uniqueCount="444">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="953" uniqueCount="447">
   <si>
     <t>First Name</t>
   </si>
@@ -1352,6 +1352,15 @@
   </si>
   <si>
     <t>Sexual Orientation</t>
+  </si>
+  <si>
+    <t>Race Unknown</t>
+  </si>
+  <si>
+    <t>Race Other</t>
+  </si>
+  <si>
+    <t>Race Refused to Answer</t>
   </si>
 </sst>
 </file>
@@ -1704,10 +1713,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:CU12"/>
+  <dimension ref="A1:CX12"/>
   <sheetViews>
-    <sheetView tabSelected="1" showOutlineSymbols="0" showWhiteSpace="0" topLeftCell="CD1" workbookViewId="0">
-      <selection activeCell="CI4" sqref="CI4"/>
+    <sheetView tabSelected="1" showOutlineSymbols="0" showWhiteSpace="0" topLeftCell="CR1" workbookViewId="0">
+      <selection activeCell="CX4" sqref="CX4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
@@ -1794,11 +1803,11 @@
     <col min="80" max="80" width="35.1640625" bestFit="1" customWidth="1"/>
     <col min="81" max="81" width="28.6640625" bestFit="1" customWidth="1"/>
     <col min="82" max="82" width="24.1640625" bestFit="1" customWidth="1"/>
-    <col min="83" max="83" width="38" bestFit="1" customWidth="1"/>
+    <col min="83" max="83" width="38.6640625" bestFit="1" customWidth="1"/>
     <col min="84" max="84" width="14.33203125" bestFit="1" customWidth="1"/>
     <col min="85" max="85" width="11.5" bestFit="1" customWidth="1"/>
     <col min="86" max="86" width="18.83203125" bestFit="1" customWidth="1"/>
-    <col min="87" max="87" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="87" max="87" width="12.1640625" bestFit="1" customWidth="1"/>
     <col min="88" max="88" width="14.5" bestFit="1" customWidth="1"/>
     <col min="89" max="89" width="27.33203125" bestFit="1" customWidth="1"/>
     <col min="90" max="90" width="16" bestFit="1" customWidth="1"/>
@@ -1808,10 +1817,16 @@
     <col min="94" max="94" width="16" bestFit="1" customWidth="1"/>
     <col min="95" max="95" width="12" bestFit="1" customWidth="1"/>
     <col min="96" max="96" width="26.1640625" bestFit="1" customWidth="1"/>
-    <col min="97" max="97" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="97" max="97" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="98" max="98" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="99" max="99" width="16" bestFit="1" customWidth="1"/>
+    <col min="100" max="100" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="101" max="101" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="102" max="102" width="21.83203125" bestFit="1" customWidth="1"/>
+    <col min="103" max="103" width="22.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:99" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:102" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2109,8 +2124,17 @@
       <c r="CU1" t="s">
         <v>443</v>
       </c>
+      <c r="CV1" t="s">
+        <v>445</v>
+      </c>
+      <c r="CW1" t="s">
+        <v>444</v>
+      </c>
+      <c r="CX1" t="s">
+        <v>446</v>
+      </c>
     </row>
-    <row r="2" spans="1:99" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:102" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
         <v>85</v>
       </c>
@@ -2391,7 +2415,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="3" spans="1:99" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:102" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
         <v>118</v>
       </c>
@@ -2672,7 +2696,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="4" spans="1:99" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:102" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
         <v>142</v>
       </c>
@@ -2953,7 +2977,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:99" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:102" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
         <v>163</v>
       </c>
@@ -3189,7 +3213,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="6" spans="1:99" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:102" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
         <v>176</v>
       </c>
@@ -3443,7 +3467,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="7" spans="1:99" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:102" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
         <v>197</v>
       </c>
@@ -3700,7 +3724,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="8" spans="1:99" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:102" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
         <v>216</v>
       </c>
@@ -3957,7 +3981,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="9" spans="1:99" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:102" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
         <v>235</v>
       </c>
@@ -4238,7 +4262,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="10" spans="1:99" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:102" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
         <v>251</v>
       </c>
@@ -4519,7 +4543,7 @@
         <v>9999</v>
       </c>
     </row>
-    <row r="11" spans="1:99" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:102" x14ac:dyDescent="0.15">
       <c r="A11" t="s">
         <v>271</v>
       </c>
@@ -4776,7 +4800,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="12" spans="1:99" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:102" x14ac:dyDescent="0.15">
       <c r="A12" t="s">
         <v>293</v>
       </c>

</xml_diff>